<commit_message>
Created console app for evaluating expressions.
</commit_message>
<xml_diff>
--- a/TextParserTest/TestData/TokeniserTestData.xlsx
+++ b/TextParserTest/TestData/TokeniserTestData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="13425"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="13860"/>
   </bookViews>
   <sheets>
     <sheet name="TokeniserTestData" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="39">
   <si>
     <t>Input</t>
   </si>
@@ -57,13 +57,85 @@
     <t>CONTAINS:((1|2|3)|1)</t>
   </si>
   <si>
-    <t>true</t>
-  </si>
-  <si>
     <t>CONTAINS:((1|2|3)|4)</t>
   </si>
   <si>
-    <t>false</t>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
+  </si>
+  <si>
+    <t>True</t>
+  </si>
+  <si>
+    <t>False</t>
+  </si>
+  <si>
+    <t>(1|2|3|4)#(1|3)</t>
+  </si>
+  <si>
+    <t>(2|4)</t>
+  </si>
+  <si>
+    <t>RANGE:(1|7|3)</t>
+  </si>
+  <si>
+    <t>(1|4|7)</t>
+  </si>
+  <si>
+    <t>(1|2|3|4|5)</t>
+  </si>
+  <si>
+    <t>REVERSE:(1|3|5)</t>
+  </si>
+  <si>
+    <t>(5|3|1)</t>
+  </si>
+  <si>
+    <t>RANGE:5</t>
+  </si>
+  <si>
+    <t>RANGE:(2|5)</t>
+  </si>
+  <si>
+    <t>(2|3|4|5)</t>
+  </si>
+  <si>
+    <t>COMP:(1|2|a|b|c)</t>
+  </si>
+  <si>
+    <t>COMP:(2|1|a|b|c)</t>
+  </si>
+  <si>
+    <t>COMP:(1|1|a|b|c)</t>
+  </si>
+  <si>
+    <t>COMP:(1|2|a|b)</t>
+  </si>
+  <si>
+    <t>COMP:(2|1|a|b)</t>
+  </si>
+  <si>
+    <t>COMP:(1|1|a|b)</t>
+  </si>
+  <si>
+    <t>COMP:(2|1|a)</t>
+  </si>
+  <si>
+    <t>COMP:(1|1|a)</t>
+  </si>
+  <si>
+    <t>OR:(IF:(True|False|True)|COMP:(0|4|False|False|True))</t>
+  </si>
+  <si>
+    <t>(10|8|6|4|2)</t>
+  </si>
+  <si>
+    <t>REVERSE:RANGE:10#RANGE:(0|8|2)</t>
   </si>
 </sst>
 </file>
@@ -547,9 +619,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -871,10 +944,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -896,15 +969,15 @@
         <v>11</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -945,6 +1018,126 @@
       </c>
       <c r="B8" s="1" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Improved scoping of function parameters.
</commit_message>
<xml_diff>
--- a/TextParserTest/TestData/TokeniserTestData.xlsx
+++ b/TextParserTest/TestData/TokeniserTestData.xlsx
@@ -14,12 +14,12 @@
   <sheets>
     <sheet name="TokeniserTestData" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="42">
   <si>
     <t>Input</t>
   </si>
@@ -136,6 +136,15 @@
   </si>
   <si>
     <t>REVERSE:RANGE:10#RANGE:(0|8|2)</t>
+  </si>
+  <si>
+    <t>CASE:(a|1|1|2|2|a|3)</t>
+  </si>
+  <si>
+    <t>CASE:(b|1|1|2|2|a|3)</t>
+  </si>
+  <si>
+    <t>CASE:(b|1|1|2|2|a|3|4)</t>
   </si>
 </sst>
 </file>
@@ -944,10 +953,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B23"/>
+  <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1140,6 +1149,27 @@
         <v>37</v>
       </c>
     </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B24" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B26" s="1">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>